<commit_message>
Start paying technical debt for our sins.
</commit_message>
<xml_diff>
--- a/test_files/sixteen_tests/4-genes_6-edges_artificial-data_Sigmoidal_estimation_fixb-1_fixP-1_graph_output.xlsx
+++ b/test_files/sixteen_tests/4-genes_6-edges_artificial-data_Sigmoidal_estimation_fixb-1_fixP-1_graph_output.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="60" windowWidth="25605" windowHeight="16005" tabRatio="644" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="11010" yWindow="0" windowWidth="14700" windowHeight="12435" tabRatio="644" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="39">
   <si>
     <t>CIN5</t>
   </si>
@@ -44,33 +44,12 @@
     <t>kk_max</t>
   </si>
   <si>
-    <t>SystematicName</t>
-  </si>
-  <si>
-    <t>StandardName</t>
-  </si>
-  <si>
-    <t>DegradationRate</t>
-  </si>
-  <si>
-    <t>YOR028C</t>
-  </si>
-  <si>
-    <t>YPR104C</t>
-  </si>
-  <si>
-    <t>rows genes affected/cols genes controlling</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
     <t>optimization_parameter</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>MaxIter</t>
   </si>
   <si>
@@ -83,21 +62,12 @@
     <t>TolX</t>
   </si>
   <si>
-    <t>YLR131C</t>
-  </si>
-  <si>
     <t>ACE2</t>
   </si>
   <si>
-    <t>production_rates</t>
-  </si>
-  <si>
     <t>AFT2</t>
   </si>
   <si>
-    <t>YPL202C</t>
-  </si>
-  <si>
     <t>Strain</t>
   </si>
   <si>
@@ -122,13 +92,31 @@
     <t>dcin5</t>
   </si>
   <si>
-    <t>simtime</t>
-  </si>
-  <si>
-    <t>estimateParams</t>
-  </si>
-  <si>
-    <t>makeGraphs</t>
+    <t>regulators/controllers</t>
+  </si>
+  <si>
+    <t>threshold_b</t>
+  </si>
+  <si>
+    <t>estimate_params</t>
+  </si>
+  <si>
+    <t>make_graphs</t>
+  </si>
+  <si>
+    <t>expression_timepoints</t>
+  </si>
+  <si>
+    <t>simulation_timepoints</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>production_rate</t>
+  </si>
+  <si>
+    <t>degradation_rate</t>
   </si>
   <si>
     <t>Parameter</t>
@@ -212,14 +200,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -236,6 +223,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,189 +630,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11" style="1"/>
+    <col min="1" max="1" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1"/>
       <c r="F1"/>
       <c r="G1"/>
-      <c r="H1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="B2">
         <v>0.5</v>
       </c>
-      <c r="H2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="H3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="H4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D4" s="5"/>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="H5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6" s="4"/>
-      <c r="H6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7" s="4"/>
-      <c r="H7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8" s="4"/>
-      <c r="H8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9" s="4"/>
-      <c r="H9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10" s="4"/>
-      <c r="H10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11" s="4"/>
-      <c r="H11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12" s="4"/>
-      <c r="H12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="H13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14" s="4"/>
-      <c r="H14"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15" s="4"/>
-      <c r="H15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16" s="4"/>
-      <c r="H16"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17" s="4"/>
-      <c r="H17"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18" s="4"/>
-      <c r="H18"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19" s="4"/>
-      <c r="E19" s="5"/>
-      <c r="H19"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="D19" s="5"/>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20" s="4"/>
-      <c r="H20"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21"/>
-      <c r="C21"/>
-      <c r="H21"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22"/>
-      <c r="C22"/>
-      <c r="H22"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E24" s="5"/>
+      <c r="G22"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D24" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -835,232 +791,223 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:W5"/>
+      <selection sqref="A1:V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
+        <v>26</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D1">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E1">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="F1">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="G1">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H1">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="I1">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="J1">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="K1">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="L1">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="M1">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N1">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="O1">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="P1">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="Q1">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="R1">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="S1">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="T1">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="U1">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="V1">
-        <v>1.9</v>
-      </c>
-      <c r="W1">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>-9.8415630865711395E-2</v>
       </c>
       <c r="D2">
-        <v>-9.8415630865711395E-2</v>
+        <v>-0.19421341855574617</v>
       </c>
       <c r="E2">
-        <v>-0.19421341855574617</v>
+        <v>-0.28729355925265893</v>
       </c>
       <c r="F2">
-        <v>-0.28729355925265893</v>
+        <v>-0.37756345942282005</v>
       </c>
       <c r="G2">
-        <v>-0.37756345942282005</v>
+        <v>-0.4649366493466236</v>
       </c>
       <c r="H2">
-        <v>-0.4649366493466236</v>
+        <v>-0.5493367221306048</v>
       </c>
       <c r="I2">
-        <v>-0.5493367221306048</v>
+        <v>-0.63069609006755056</v>
       </c>
       <c r="J2">
-        <v>-0.63069609006755056</v>
+        <v>-0.70895953801899125</v>
       </c>
       <c r="K2">
-        <v>-0.70895953801899125</v>
+        <v>-0.78408287327487469</v>
       </c>
       <c r="L2">
-        <v>-0.78408287327487469</v>
+        <v>-0.85603594995930821</v>
       </c>
       <c r="M2">
-        <v>-0.85603594995930821</v>
+        <v>-0.92480109285265377</v>
       </c>
       <c r="N2">
-        <v>-0.92480109285265377</v>
+        <v>-0.9903754864911255</v>
       </c>
       <c r="O2">
-        <v>-0.9903754864911255</v>
+        <v>-1.0527692995615539</v>
       </c>
       <c r="P2">
-        <v>-1.0527692995615539</v>
+        <v>-1.1120073944279283</v>
       </c>
       <c r="Q2">
-        <v>-1.1120073944279283</v>
+        <v>-1.168127143194938</v>
       </c>
       <c r="R2">
-        <v>-1.168127143194938</v>
+        <v>-1.2211794869461998</v>
       </c>
       <c r="S2">
-        <v>-1.2211794869461998</v>
+        <v>-1.2712265015727739</v>
       </c>
       <c r="T2">
-        <v>-1.2712265015727739</v>
+        <v>-1.3183419034269952</v>
       </c>
       <c r="U2">
-        <v>-1.3183419034269952</v>
+        <v>-1.3626084757375463</v>
       </c>
       <c r="V2">
-        <v>-1.3626084757375463</v>
-      </c>
-      <c r="W2">
         <v>-1.4041180953399601</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>-6.1695580472264637E-2</v>
       </c>
       <c r="D3">
-        <v>-6.1695580472264637E-2</v>
+        <v>-0.12025159100022467</v>
       </c>
       <c r="E3">
-        <v>-0.12025159100022467</v>
+        <v>-0.17570780612319539</v>
       </c>
       <c r="F3">
-        <v>-0.17570780612319539</v>
+        <v>-0.22811720726268783</v>
       </c>
       <c r="G3">
-        <v>-0.22811720726268783</v>
+        <v>-0.27754366929297497</v>
       </c>
       <c r="H3">
-        <v>-0.27754366929297497</v>
+        <v>-0.32406241829767435</v>
       </c>
       <c r="I3">
-        <v>-0.32406241829767435</v>
+        <v>-0.3677574742905928</v>
       </c>
       <c r="J3">
-        <v>-0.3677574742905928</v>
+        <v>-0.40872171608120611</v>
       </c>
       <c r="K3">
-        <v>-0.40872171608120611</v>
+        <v>-0.44705433466919547</v>
       </c>
       <c r="L3">
-        <v>-0.44705433466919547</v>
+        <v>-0.48286066269974875</v>
       </c>
       <c r="M3">
-        <v>-0.48286066269974875</v>
+        <v>-0.51624977105786596</v>
       </c>
       <c r="N3">
-        <v>-0.51624977105786596</v>
+        <v>-0.54733420681301193</v>
       </c>
       <c r="O3">
-        <v>-0.54733420681301193</v>
+        <v>-0.57622783863033211</v>
       </c>
       <c r="P3">
-        <v>-0.57622783863033211</v>
+        <v>-0.60304561487847708</v>
       </c>
       <c r="Q3">
-        <v>-0.60304561487847708</v>
+        <v>-0.62790172449432446</v>
       </c>
       <c r="R3">
-        <v>-0.62790172449432446</v>
+        <v>-0.65090944702397735</v>
       </c>
       <c r="S3">
-        <v>-0.65090944702397735</v>
+        <v>-0.67217965509992694</v>
       </c>
       <c r="T3">
-        <v>-0.67217965509992694</v>
+        <v>-0.69182079016701059</v>
       </c>
       <c r="U3">
-        <v>-0.69182079016701059</v>
+        <v>-0.70993769854923061</v>
       </c>
       <c r="V3">
-        <v>-0.70993769854923061</v>
-      </c>
-      <c r="W3">
         <v>-0.72663170963117274</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
@@ -1123,78 +1070,72 @@
       <c r="V4">
         <v>0</v>
       </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>-3.908229913513931E-2</v>
       </c>
       <c r="D5">
-        <v>-3.908229913513931E-2</v>
+        <v>-7.6100322098197407E-2</v>
       </c>
       <c r="E5">
-        <v>-7.6100322098197407E-2</v>
+        <v>-0.11112054431760732</v>
       </c>
       <c r="F5">
-        <v>-0.11112054431760732</v>
+        <v>-0.14421175778249326</v>
       </c>
       <c r="G5">
-        <v>-0.14421175778249326</v>
+        <v>-0.17544416984513003</v>
       </c>
       <c r="H5">
-        <v>-0.17544416984513003</v>
+        <v>-0.2048894472936392</v>
       </c>
       <c r="I5">
-        <v>-0.2048894472936392</v>
+        <v>-0.23261983766255628</v>
       </c>
       <c r="J5">
-        <v>-0.23261983766255628</v>
+        <v>-0.25870816923429668</v>
       </c>
       <c r="K5">
-        <v>-0.25870816923429668</v>
+        <v>-0.28322705890386018</v>
       </c>
       <c r="L5">
-        <v>-0.28322705890386018</v>
+        <v>-0.3062489023647269</v>
       </c>
       <c r="M5">
-        <v>-0.3062489023647269</v>
+        <v>-0.32784518455607942</v>
       </c>
       <c r="N5">
-        <v>-0.32784518455607942</v>
+        <v>-0.34808648361082384</v>
       </c>
       <c r="O5">
-        <v>-0.34808648361082384</v>
+        <v>-0.36704189081996774</v>
       </c>
       <c r="P5">
-        <v>-0.36704189081996774</v>
+        <v>-0.38477904199353069</v>
       </c>
       <c r="Q5">
-        <v>-0.38477904199353069</v>
+        <v>-0.40136364593067475</v>
       </c>
       <c r="R5">
-        <v>-0.40136364593067475</v>
+        <v>-0.41685954866879965</v>
       </c>
       <c r="S5">
-        <v>-0.41685954866879965</v>
+        <v>-0.43132836339590414</v>
       </c>
       <c r="T5">
-        <v>-0.43132836339590414</v>
+        <v>-0.44482956705563848</v>
       </c>
       <c r="U5">
-        <v>-0.44482956705563848</v>
+        <v>-0.45742022068355997</v>
       </c>
       <c r="V5">
-        <v>-0.45742022068355997</v>
-      </c>
-      <c r="W5">
         <v>-0.46915508490039931</v>
       </c>
     </row>
@@ -1205,63 +1146,57 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
+        <v>26</v>
+      </c>
+      <c r="B1">
+        <v>0.4</v>
       </c>
       <c r="C1">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D1">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="E1">
-        <v>1.2</v>
-      </c>
-      <c r="F1">
         <v>1.6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>6.7986997775525911E-17</v>
       </c>
       <c r="C2">
-        <v>6.7986997775525911E-17</v>
+        <v>1.3597399555105182E-16</v>
       </c>
       <c r="D2">
-        <v>1.3597399555105182E-16</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>3.3993498887762956E-17</v>
       </c>
       <c r="C3">
-        <v>3.3993498887762956E-17</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1269,15 +1204,12 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
@@ -1289,16 +1221,13 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1307,9 +1236,6 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
         <v>0</v>
       </c>
     </row>
@@ -1320,63 +1246,57 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
+        <v>26</v>
+      </c>
+      <c r="B1">
+        <v>0.4</v>
       </c>
       <c r="C1">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D1">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="E1">
-        <v>1.2</v>
-      </c>
-      <c r="F1">
         <v>1.6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>6.7986997775525911E-17</v>
       </c>
       <c r="C2">
-        <v>6.7986997775525911E-17</v>
+        <v>1.3597399555105182E-16</v>
       </c>
       <c r="D2">
-        <v>1.3597399555105182E-16</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>3.3993498887762956E-17</v>
       </c>
       <c r="C3">
-        <v>3.3993498887762956E-17</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1384,15 +1304,12 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
@@ -1404,16 +1321,13 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1422,9 +1336,6 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
         <v>0</v>
       </c>
     </row>
@@ -1445,13 +1356,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1462,7 +1373,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0.48106324262704242</v>
@@ -1479,7 +1390,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1545,15 +1456,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>2.8800449743390965E-5</v>
@@ -1561,7 +1472,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0.50509378836733443</v>
@@ -1569,7 +1480,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B4">
         <v>1.2133358649639586E-33</v>
@@ -1577,7 +1488,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B5">
         <v>304</v>
@@ -1585,23 +1496,23 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>7.2017297682751277E-5</v>
@@ -1612,7 +1523,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>6.2184419952668641E-6</v>
@@ -1650,159 +1561,126 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11" style="1"/>
+    <col min="1" max="1" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19"/>
       <c r="B19"/>
-      <c r="C19"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20"/>
       <c r="B20"/>
-      <c r="C20"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21"/>
-      <c r="C21"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22"/>
-      <c r="C22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -1814,20 +1692,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
+        <v>26</v>
+      </c>
+      <c r="B1" s="10">
+        <v>0.4</v>
       </c>
       <c r="C1" s="11">
         <v>0.4</v>
@@ -1836,7 +1714,7 @@
         <v>0.4</v>
       </c>
       <c r="E1" s="13">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="F1" s="14">
         <v>0.8</v>
@@ -1845,16 +1723,16 @@
         <v>0.8</v>
       </c>
       <c r="H1" s="16">
-        <v>0.8</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="I1" s="17">
         <v>1.2000000000000002</v>
       </c>
       <c r="J1" s="18">
-        <v>1.2000000000000002</v>
+        <v>1.2</v>
       </c>
       <c r="K1" s="19">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="L1" s="20">
         <v>1.6</v>
@@ -1862,17 +1740,14 @@
       <c r="M1" s="21">
         <v>1.6</v>
       </c>
-      <c r="N1" s="22">
-        <v>1.6</v>
-      </c>
-      <c r="O1" s="7"/>
-    </row>
-    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="B2" s="10">
+        <v>-0.37633430629205178</v>
       </c>
       <c r="C2" s="11">
         <v>-0.37633430629205178</v>
@@ -1881,7 +1756,7 @@
         <v>-0.37633430629205178</v>
       </c>
       <c r="E2" s="13">
-        <v>-0.37633430629205178</v>
+        <v>-0.70666646734338179</v>
       </c>
       <c r="F2" s="14">
         <v>-0.70666646734338179</v>
@@ -1890,7 +1765,7 @@
         <v>-0.70666646734338179</v>
       </c>
       <c r="H2" s="16">
-        <v>-0.70666646734338179</v>
+        <v>-0.98723929967009216</v>
       </c>
       <c r="I2" s="17">
         <v>-0.98723929967009216</v>
@@ -1899,7 +1774,7 @@
         <v>-0.98723929967009216</v>
       </c>
       <c r="K2" s="19">
-        <v>-0.98723929967009216</v>
+        <v>-1.2174432654761544</v>
       </c>
       <c r="L2" s="20">
         <v>-1.2174432654761544</v>
@@ -1907,16 +1782,13 @@
       <c r="M2" s="21">
         <v>-1.2174432654761544</v>
       </c>
-      <c r="N2" s="22">
-        <v>-1.2174432654761544</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="10">
+        <v>-0.22771865423983556</v>
       </c>
       <c r="C3" s="11">
         <v>-0.22771865423983556</v>
@@ -1925,7 +1797,7 @@
         <v>-0.22771865423983556</v>
       </c>
       <c r="E3" s="13">
-        <v>-0.22771865423983556</v>
+        <v>-0.40801774302656463</v>
       </c>
       <c r="F3" s="14">
         <v>-0.40801774302656463</v>
@@ -1934,7 +1806,7 @@
         <v>-0.40801774302656463</v>
       </c>
       <c r="H3" s="16">
-        <v>-0.40801774302656463</v>
+        <v>-0.5464126532391167</v>
       </c>
       <c r="I3" s="17">
         <v>-0.5464126532391167</v>
@@ -1943,7 +1815,7 @@
         <v>-0.5464126532391167</v>
       </c>
       <c r="K3" s="19">
-        <v>-0.5464126532391167</v>
+        <v>-0.64984386018298912</v>
       </c>
       <c r="L3" s="20">
         <v>-0.64984386018298912</v>
@@ -1951,16 +1823,13 @@
       <c r="M3" s="21">
         <v>-0.64984386018298912</v>
       </c>
-      <c r="N3" s="22">
-        <v>-0.64984386018298912</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0.26929382132237512</v>
       </c>
       <c r="C4" s="11">
         <v>0.26929382132237512</v>
@@ -1969,7 +1838,7 @@
         <v>0.26929382132237512</v>
       </c>
       <c r="E4" s="13">
-        <v>0.26929382132237512</v>
+        <v>0.41593537248224854</v>
       </c>
       <c r="F4" s="14">
         <v>0.41593537248224854</v>
@@ -1978,7 +1847,7 @@
         <v>0.41593537248224854</v>
       </c>
       <c r="H4" s="16">
-        <v>0.41593537248224854</v>
+        <v>0.49751163358969142</v>
       </c>
       <c r="I4" s="17">
         <v>0.49751163358969142</v>
@@ -1987,7 +1856,7 @@
         <v>0.49751163358969142</v>
       </c>
       <c r="K4" s="19">
-        <v>0.49751163358969142</v>
+        <v>0.54159993841241572</v>
       </c>
       <c r="L4" s="20">
         <v>0.54159993841241572</v>
@@ -1995,16 +1864,13 @@
       <c r="M4" s="21">
         <v>0.54159993841241572</v>
       </c>
-      <c r="N4" s="22">
-        <v>0.54159993841241572</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B5" s="10">
+        <v>-0.29093615522070321</v>
       </c>
       <c r="C5" s="11">
         <v>-0.29093615522070321</v>
@@ -2013,7 +1879,7 @@
         <v>-0.29093615522070321</v>
       </c>
       <c r="E5" s="13">
-        <v>-0.29093615522070321</v>
+        <v>-0.57977180156386388</v>
       </c>
       <c r="F5" s="14">
         <v>-0.57977180156386388</v>
@@ -2022,7 +1888,7 @@
         <v>-0.57977180156386388</v>
       </c>
       <c r="H5" s="16">
-        <v>-0.57977180156386388</v>
+        <v>-0.85583465653557034</v>
       </c>
       <c r="I5" s="17">
         <v>-0.85583465653557034</v>
@@ -2031,7 +1897,7 @@
         <v>-0.85583465653557034</v>
       </c>
       <c r="K5" s="19">
-        <v>-0.85583465653557034</v>
+        <v>-1.1097262320569594</v>
       </c>
       <c r="L5" s="20">
         <v>-1.1097262320569594</v>
@@ -2039,37 +1905,34 @@
       <c r="M5" s="21">
         <v>-1.1097262320569594</v>
       </c>
-      <c r="N5" s="22">
-        <v>-1.1097262320569594</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G6" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J10" s="2"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G12" s="2"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I14" s="2"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="I18" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="H18" s="2"/>
+      <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="F20" s="2"/>
-      <c r="M20" s="2"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="E20" s="2"/>
+      <c r="L20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2081,282 +1944,267 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="10">
+        <v>26</v>
+      </c>
+      <c r="B1" s="9">
         <v>0.4</v>
       </c>
-      <c r="D1" s="10">
+      <c r="C1" s="9">
         <v>0.4</v>
       </c>
-      <c r="E1" s="10">
+      <c r="D1" s="9">
         <v>0.4</v>
       </c>
-      <c r="F1" s="10">
+      <c r="E1" s="9">
         <v>0.8</v>
       </c>
-      <c r="G1" s="10">
+      <c r="F1" s="9">
         <v>0.8</v>
       </c>
-      <c r="H1" s="10">
+      <c r="G1" s="9">
         <v>0.8</v>
       </c>
-      <c r="I1" s="10">
+      <c r="H1" s="9">
         <v>1.2000000000000002</v>
       </c>
-      <c r="J1" s="10">
+      <c r="I1" s="9">
         <v>1.2000000000000002</v>
       </c>
-      <c r="K1" s="10">
+      <c r="J1" s="9">
         <v>1.2</v>
       </c>
-      <c r="L1" s="10">
+      <c r="K1" s="9">
         <v>1.6</v>
       </c>
-      <c r="M1" s="10">
+      <c r="L1" s="9">
         <v>1.6</v>
       </c>
-      <c r="N1" s="10">
+      <c r="M1" s="9">
         <v>1.6</v>
       </c>
-      <c r="O1" s="7"/>
-    </row>
-    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="10">
+        <v>10</v>
+      </c>
+      <c r="B2" s="9">
         <v>-0.37633430629205178</v>
       </c>
-      <c r="D2" s="10">
+      <c r="C2" s="9">
         <v>-0.37633430629205178</v>
       </c>
-      <c r="E2" s="10">
+      <c r="D2" s="9">
         <v>-0.37633430629205178</v>
       </c>
-      <c r="F2" s="10">
+      <c r="E2" s="9">
         <v>-0.70666646734338179</v>
       </c>
-      <c r="G2" s="10">
+      <c r="F2" s="9">
         <v>-0.70666646734338179</v>
       </c>
-      <c r="H2" s="10">
+      <c r="G2" s="9">
         <v>-0.70666646734338179</v>
       </c>
-      <c r="I2" s="10">
+      <c r="H2" s="9">
         <v>-0.98723929967009216</v>
       </c>
-      <c r="J2" s="10">
+      <c r="I2" s="9">
         <v>-0.98723929967009216</v>
       </c>
-      <c r="K2" s="10">
+      <c r="J2" s="9">
         <v>-0.98723929967009216</v>
       </c>
-      <c r="L2" s="10">
+      <c r="K2" s="9">
         <v>-1.2174432654761544</v>
       </c>
-      <c r="M2" s="10">
+      <c r="L2" s="9">
         <v>-1.2174432654761544</v>
       </c>
-      <c r="N2" s="10">
+      <c r="M2" s="9">
         <v>-1.2174432654761544</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="10">
+        <v>11</v>
+      </c>
+      <c r="B3" s="9">
         <v>-0.22771865423983556</v>
       </c>
-      <c r="D3" s="10">
+      <c r="C3" s="9">
         <v>-0.22771865423983556</v>
       </c>
-      <c r="E3" s="10">
+      <c r="D3" s="9">
         <v>-0.22771865423983556</v>
       </c>
-      <c r="F3" s="10">
+      <c r="E3" s="9">
         <v>-0.40801774302656463</v>
       </c>
-      <c r="G3" s="10">
+      <c r="F3" s="9">
         <v>-0.40801774302656463</v>
       </c>
-      <c r="H3" s="10">
+      <c r="G3" s="9">
         <v>-0.40801774302656463</v>
       </c>
-      <c r="I3" s="10">
+      <c r="H3" s="9">
         <v>-0.5464126532391167</v>
       </c>
-      <c r="J3" s="10">
+      <c r="I3" s="9">
         <v>-0.5464126532391167</v>
       </c>
-      <c r="K3" s="10">
+      <c r="J3" s="9">
         <v>-0.5464126532391167</v>
       </c>
-      <c r="L3" s="10">
+      <c r="K3" s="9">
         <v>-0.64984386018298912</v>
       </c>
-      <c r="M3" s="10">
+      <c r="L3" s="9">
         <v>-0.64984386018298912</v>
       </c>
-      <c r="N3" s="10">
+      <c r="M3" s="9">
         <v>-0.64984386018298912</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="10">
-        <v>0</v>
-      </c>
-      <c r="D4" s="10">
-        <v>0</v>
-      </c>
-      <c r="E4" s="10">
-        <v>0</v>
-      </c>
-      <c r="F4" s="10">
-        <v>0</v>
-      </c>
-      <c r="G4" s="10">
-        <v>0</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0</v>
-      </c>
-      <c r="I4" s="10">
-        <v>0</v>
-      </c>
-      <c r="J4" s="10">
-        <v>0</v>
-      </c>
-      <c r="K4" s="10">
-        <v>0</v>
-      </c>
-      <c r="L4" s="10">
-        <v>0</v>
-      </c>
-      <c r="M4" s="10">
-        <v>0</v>
-      </c>
-      <c r="N4" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="10">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9">
         <v>-0.13932150464649004</v>
       </c>
-      <c r="D5" s="10">
+      <c r="C5" s="9">
         <v>-0.13932150464649004</v>
       </c>
-      <c r="E5" s="10">
+      <c r="D5" s="9">
         <v>-0.13932150464649004</v>
       </c>
-      <c r="F5" s="10">
+      <c r="E5" s="9">
         <v>-0.24985173044541253</v>
       </c>
-      <c r="G5" s="10">
+      <c r="F5" s="9">
         <v>-0.24985173044541253</v>
       </c>
-      <c r="H5" s="10">
+      <c r="G5" s="9">
         <v>-0.24985173044541253</v>
       </c>
-      <c r="I5" s="10">
+      <c r="H5" s="9">
         <v>-0.33614068837409528</v>
       </c>
-      <c r="J5" s="10">
+      <c r="I5" s="9">
         <v>-0.33614068837409528</v>
       </c>
-      <c r="K5" s="10">
+      <c r="J5" s="9">
         <v>-0.33614068837409528</v>
       </c>
-      <c r="L5" s="10">
+      <c r="K5" s="9">
         <v>-0.40259011361710589</v>
       </c>
-      <c r="M5" s="10">
+      <c r="L5" s="9">
         <v>-0.40259011361710589</v>
       </c>
-      <c r="N5" s="10">
+      <c r="M5" s="9">
         <v>-0.40259011361710589</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="L7" s="2"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K7" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="N10" s="2"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F11" s="2"/>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C15" s="2"/>
-    </row>
-    <row r="18" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="G18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="I19" s="2"/>
-      <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="I20" s="2"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="22" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="L22" s="2"/>
-      <c r="N22" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="18" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F18" s="2"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="H19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="H20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="22" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="K22" s="2"/>
+      <c r="M22" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2370,12 +2218,12 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.25" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5.125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.75" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.875" style="4" bestFit="1" customWidth="1"/>
@@ -2396,14 +2244,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>9</v>
+      <c r="A1" s="23" t="s">
+        <v>20</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>0</v>
@@ -2413,8 +2261,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>18</v>
+      <c r="A2" t="s">
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -2430,8 +2278,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>20</v>
+      <c r="A3" t="s">
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -2447,7 +2295,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4">
@@ -2464,7 +2312,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="4">
@@ -2493,7 +2341,7 @@
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2518,14 +2366,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>9</v>
+      <c r="A1" s="23" t="s">
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2553,7 +2401,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -2570,7 +2418,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -2632,7 +2480,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2642,22 +2490,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2678,7 +2526,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>1000000</v>
@@ -2686,7 +2534,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>1.0000000000000001E-5</v>
@@ -2694,7 +2542,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>1000000</v>
@@ -2702,7 +2550,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>1.0000000000000001E-5</v>
@@ -2710,49 +2558,49 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="9">
+        <v>18</v>
+      </c>
+      <c r="B8" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="9">
+        <v>22</v>
+      </c>
+      <c r="B9" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="9">
+        <v>23</v>
+      </c>
+      <c r="B10" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="9">
+        <v>15</v>
+      </c>
+      <c r="B11" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="9">
+        <v>16</v>
+      </c>
+      <c r="B12" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="9">
+        <v>24</v>
+      </c>
+      <c r="B13" s="8">
         <v>0.4</v>
       </c>
       <c r="C13">
@@ -2767,20 +2615,20 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="8">
+        <v>17</v>
+      </c>
+      <c r="B15" s="7">
         <v>3</v>
       </c>
       <c r="C15">
@@ -2789,9 +2637,9 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="8">
+        <v>13</v>
+      </c>
+      <c r="B16" s="7">
         <v>0</v>
       </c>
       <c r="C16">
@@ -2800,7 +2648,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2878,20 +2726,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
+      <c r="A1" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2899,7 +2750,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2935,366 +2786,351 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:W5"/>
+      <selection sqref="A1:V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
+        <v>26</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D1">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E1">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="F1">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="G1">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H1">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="I1">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="J1">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="K1">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="L1">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="M1">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N1">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="O1">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="P1">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="Q1">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="R1">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="S1">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="T1">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="U1">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="V1">
-        <v>1.9</v>
-      </c>
-      <c r="W1">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>-9.8415630865711395E-2</v>
       </c>
       <c r="D2">
-        <v>-9.8415630865711395E-2</v>
+        <v>-0.19421341855574617</v>
       </c>
       <c r="E2">
-        <v>-0.19421341855574617</v>
+        <v>-0.28729355925265893</v>
       </c>
       <c r="F2">
-        <v>-0.28729355925265893</v>
+        <v>-0.37756345942282005</v>
       </c>
       <c r="G2">
-        <v>-0.37756345942282005</v>
+        <v>-0.4649366493466236</v>
       </c>
       <c r="H2">
-        <v>-0.4649366493466236</v>
+        <v>-0.5493367221306048</v>
       </c>
       <c r="I2">
-        <v>-0.5493367221306048</v>
+        <v>-0.63069609006755056</v>
       </c>
       <c r="J2">
-        <v>-0.63069609006755056</v>
+        <v>-0.70895953801899125</v>
       </c>
       <c r="K2">
-        <v>-0.70895953801899125</v>
+        <v>-0.78408287327487469</v>
       </c>
       <c r="L2">
-        <v>-0.78408287327487469</v>
+        <v>-0.85603594995930821</v>
       </c>
       <c r="M2">
-        <v>-0.85603594995930821</v>
+        <v>-0.92480109285265377</v>
       </c>
       <c r="N2">
-        <v>-0.92480109285265377</v>
+        <v>-0.9903754864911255</v>
       </c>
       <c r="O2">
-        <v>-0.9903754864911255</v>
+        <v>-1.0527692995615539</v>
       </c>
       <c r="P2">
-        <v>-1.0527692995615539</v>
+        <v>-1.1120073944279283</v>
       </c>
       <c r="Q2">
-        <v>-1.1120073944279283</v>
+        <v>-1.168127143194938</v>
       </c>
       <c r="R2">
-        <v>-1.168127143194938</v>
+        <v>-1.2211794869461998</v>
       </c>
       <c r="S2">
-        <v>-1.2211794869461998</v>
+        <v>-1.2712265015727739</v>
       </c>
       <c r="T2">
-        <v>-1.2712265015727739</v>
+        <v>-1.3183419034269952</v>
       </c>
       <c r="U2">
-        <v>-1.3183419034269952</v>
+        <v>-1.3626084757375463</v>
       </c>
       <c r="V2">
-        <v>-1.3626084757375463</v>
-      </c>
-      <c r="W2">
         <v>-1.4041180953399601</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>-6.1695580472264637E-2</v>
       </c>
       <c r="D3">
-        <v>-6.1695580472264637E-2</v>
+        <v>-0.12025159100022467</v>
       </c>
       <c r="E3">
-        <v>-0.12025159100022467</v>
+        <v>-0.17570780612319539</v>
       </c>
       <c r="F3">
-        <v>-0.17570780612319539</v>
+        <v>-0.22811720726268783</v>
       </c>
       <c r="G3">
-        <v>-0.22811720726268783</v>
+        <v>-0.27754366929297497</v>
       </c>
       <c r="H3">
-        <v>-0.27754366929297497</v>
+        <v>-0.32406241829767435</v>
       </c>
       <c r="I3">
-        <v>-0.32406241829767435</v>
+        <v>-0.3677574742905928</v>
       </c>
       <c r="J3">
-        <v>-0.3677574742905928</v>
+        <v>-0.40872171608120611</v>
       </c>
       <c r="K3">
-        <v>-0.40872171608120611</v>
+        <v>-0.44705433466919547</v>
       </c>
       <c r="L3">
-        <v>-0.44705433466919547</v>
+        <v>-0.48286066269974875</v>
       </c>
       <c r="M3">
-        <v>-0.48286066269974875</v>
+        <v>-0.51624977105786596</v>
       </c>
       <c r="N3">
-        <v>-0.51624977105786596</v>
+        <v>-0.54733420681301193</v>
       </c>
       <c r="O3">
-        <v>-0.54733420681301193</v>
+        <v>-0.57622783863033211</v>
       </c>
       <c r="P3">
-        <v>-0.57622783863033211</v>
+        <v>-0.60304561487847708</v>
       </c>
       <c r="Q3">
-        <v>-0.60304561487847708</v>
+        <v>-0.62790172449432446</v>
       </c>
       <c r="R3">
-        <v>-0.62790172449432446</v>
+        <v>-0.65090944702397735</v>
       </c>
       <c r="S3">
-        <v>-0.65090944702397735</v>
+        <v>-0.67217965509992694</v>
       </c>
       <c r="T3">
-        <v>-0.67217965509992694</v>
+        <v>-0.69182079016701059</v>
       </c>
       <c r="U3">
-        <v>-0.69182079016701059</v>
+        <v>-0.70993769854923061</v>
       </c>
       <c r="V3">
-        <v>-0.70993769854923061</v>
-      </c>
-      <c r="W3">
         <v>-0.72663170963117274</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>7.7639211246089856E-2</v>
       </c>
       <c r="D4">
-        <v>7.7639211246089856E-2</v>
+        <v>0.14472504847124545</v>
       </c>
       <c r="E4">
-        <v>0.14472504847124545</v>
+        <v>0.20302845631162525</v>
       </c>
       <c r="F4">
-        <v>0.20302845631162525</v>
+        <v>0.25393703305900761</v>
       </c>
       <c r="G4">
-        <v>0.25393703305900761</v>
+        <v>0.29855749804680276</v>
       </c>
       <c r="H4">
-        <v>0.29855749804680276</v>
+        <v>0.33778725020176992</v>
       </c>
       <c r="I4">
-        <v>0.33778725020176992</v>
+        <v>0.37236316575682393</v>
       </c>
       <c r="J4">
-        <v>0.37236316575682393</v>
+        <v>0.40289805134748413</v>
       </c>
       <c r="K4">
-        <v>0.40289805134748413</v>
+        <v>0.42990615842655922</v>
       </c>
       <c r="L4">
-        <v>0.42990615842655922</v>
+        <v>0.45382343385594281</v>
       </c>
       <c r="M4">
-        <v>0.45382343385594281</v>
+        <v>0.47502183439538348</v>
       </c>
       <c r="N4">
-        <v>0.47502183439538348</v>
+        <v>0.49382137920476943</v>
       </c>
       <c r="O4">
-        <v>0.49382137920476943</v>
+        <v>0.51049863814483687</v>
       </c>
       <c r="P4">
-        <v>0.51049863814483687</v>
+        <v>0.52529432069690762</v>
       </c>
       <c r="Q4">
-        <v>0.52529432069690762</v>
+        <v>0.53841853990578037</v>
       </c>
       <c r="R4">
-        <v>0.53841853990578037</v>
+        <v>0.55005582014022014</v>
       </c>
       <c r="S4">
-        <v>0.55005582014022014</v>
+        <v>0.56036848504203962</v>
       </c>
       <c r="T4">
-        <v>0.56036848504203962</v>
+        <v>0.56950009509884514</v>
       </c>
       <c r="U4">
-        <v>0.56950009509884514</v>
+        <v>0.5775776982012687</v>
       </c>
       <c r="V4">
-        <v>0.5775776982012687</v>
-      </c>
-      <c r="W4">
         <v>0.58471425529729304</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>-7.2980348206178186E-2</v>
       </c>
       <c r="D5">
-        <v>-7.2980348206178186E-2</v>
+        <v>-0.14602894484549481</v>
       </c>
       <c r="E5">
-        <v>-0.14602894484549481</v>
+        <v>-0.21903139734662802</v>
       </c>
       <c r="F5">
-        <v>-0.21903139734662802</v>
+        <v>-0.29186239678888332</v>
       </c>
       <c r="G5">
-        <v>-0.29186239678888332</v>
+        <v>-0.36438997011105467</v>
       </c>
       <c r="H5">
-        <v>-0.36438997011105467</v>
+        <v>-0.4364779942273927</v>
       </c>
       <c r="I5">
-        <v>-0.4364779942273927</v>
+        <v>-0.50798923604580948</v>
       </c>
       <c r="J5">
-        <v>-0.50798923604580948</v>
+        <v>-0.57878698389398842</v>
       </c>
       <c r="K5">
-        <v>-0.57878698389398842</v>
+        <v>-0.64873713558317958</v>
       </c>
       <c r="L5">
-        <v>-0.64873713558317958</v>
+        <v>-0.71770927071314694</v>
       </c>
       <c r="M5">
-        <v>-0.71770927071314694</v>
+        <v>-0.78557807685706316</v>
       </c>
       <c r="N5">
-        <v>-0.78557807685706316</v>
+        <v>-0.85222410981586638</v>
       </c>
       <c r="O5">
-        <v>-0.85222410981586638</v>
+        <v>-0.91753476827466685</v>
       </c>
       <c r="P5">
-        <v>-0.91753476827466685</v>
+        <v>-0.98140489075521198</v>
       </c>
       <c r="Q5">
-        <v>-0.98140489075521198</v>
+        <v>-1.0437374061694207</v>
       </c>
       <c r="R5">
-        <v>-1.0437374061694207</v>
+        <v>-1.104443833661269</v>
       </c>
       <c r="S5">
-        <v>-1.104443833661269</v>
+        <v>-1.1634446725731808</v>
       </c>
       <c r="T5">
-        <v>-1.1634446725731808</v>
+        <v>-1.2206698155918494</v>
       </c>
       <c r="U5">
-        <v>-1.2206698155918494</v>
+        <v>-1.2760587016112892</v>
       </c>
       <c r="V5">
-        <v>-1.2760587016112892</v>
-      </c>
-      <c r="W5">
         <v>-1.3295606106401805</v>
       </c>
     </row>

</xml_diff>